<commit_message>
Project Ready For Submission
Getting the project ready for submission. Added documentation and
made sure names were needed where credit is due. Removed checkstyle errors.
Made sure the log file was also added.
</commit_message>
<xml_diff>
--- a/Documentation/Sprint Backlog.xlsx
+++ b/Documentation/Sprint Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angli\OneDrive\Desktop\eclipse-workspace\TextAdventureGame2.0\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jb00645\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE6118A-9550-413E-8596-A27F9DA67390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B95FCC4-B7A9-4055-8EFE-0C42B0D9C5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29025" yWindow="-2775" windowWidth="30930" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41340" yWindow="0" windowWidth="19200" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>Task Manager / Dev</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Amount Remaining After…</t>
   </si>
   <si>
-    <t>Day 1</t>
-  </si>
-  <si>
     <t>Day 2</t>
   </si>
   <si>
@@ -71,30 +68,6 @@
     <t>Day 7</t>
   </si>
   <si>
-    <t>Day 8</t>
-  </si>
-  <si>
-    <t>Day 9</t>
-  </si>
-  <si>
-    <t>Day 10</t>
-  </si>
-  <si>
-    <t>Day 11</t>
-  </si>
-  <si>
-    <t>Day 12</t>
-  </si>
-  <si>
-    <t>Day 13</t>
-  </si>
-  <si>
-    <t>Day 14</t>
-  </si>
-  <si>
-    <t>Day 15</t>
-  </si>
-  <si>
     <t>Implement NPC</t>
   </si>
   <si>
@@ -125,15 +98,6 @@
     <t>Load Items</t>
   </si>
   <si>
-    <t>Map Gen (Location)</t>
-  </si>
-  <si>
-    <t>Map Gen (NPC)</t>
-  </si>
-  <si>
-    <t>Map Gen (Item)</t>
-  </si>
-  <si>
     <t>Estimate Totals</t>
   </si>
   <si>
@@ -146,13 +110,115 @@
     <t>Colby</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Actual Time Totals</t>
   </si>
   <si>
     <t>Actual Time</t>
+  </si>
+  <si>
+    <t>Day 1 (Monday 2)</t>
+  </si>
+  <si>
+    <t>Day 12 (Friday 13)</t>
+  </si>
+  <si>
+    <t>Refactor NPC</t>
+  </si>
+  <si>
+    <t>Date of Work</t>
+  </si>
+  <si>
+    <t>Implement NPC and Item interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jacob </t>
+  </si>
+  <si>
+    <t>Saturday 7th</t>
+  </si>
+  <si>
+    <t>Sunday 8th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load NPC </t>
+  </si>
+  <si>
+    <t>Implment NPC</t>
+  </si>
+  <si>
+    <t>Add NPC to world</t>
+  </si>
+  <si>
+    <t>Refactored Items</t>
+  </si>
+  <si>
+    <t>Implmented Items</t>
+  </si>
+  <si>
+    <t>Wednesday 4th</t>
+  </si>
+  <si>
+    <t>Tuesday 3rd</t>
+  </si>
+  <si>
+    <t>Load Items (.txt file creation)</t>
+  </si>
+  <si>
+    <t>Load NPC (.txt file creation)</t>
+  </si>
+  <si>
+    <t>Refactor Items (testing for full coverage)</t>
+  </si>
+  <si>
+    <t>Implment Items (testing for full coverage)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 8 </t>
+  </si>
+  <si>
+    <t>Day 9 (10th)</t>
+  </si>
+  <si>
+    <t>Day 10 (11th)</t>
+  </si>
+  <si>
+    <t>Day 11 (12th)</t>
+  </si>
+  <si>
+    <t>Random Map Gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday 11th </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monday 9th </t>
+  </si>
+  <si>
+    <t>Tuesday 10th</t>
+  </si>
+  <si>
+    <t>Assisting kate with NPC and Item interaction</t>
+  </si>
+  <si>
+    <t>Implement Merchant Trading with UI</t>
+  </si>
+  <si>
+    <t>Pick up Item and Refactor Drop Items</t>
+  </si>
+  <si>
+    <t>Adding NPC to World and adding some movement</t>
+  </si>
+  <si>
+    <t>Thursday 12th</t>
+  </si>
+  <si>
+    <t>Implement Merchant Logic</t>
+  </si>
+  <si>
+    <t>Checking For bug(testing game logic) and Refactoring</t>
+  </si>
+  <si>
+    <t>View Binding and Bug Fixes</t>
   </si>
 </sst>
 </file>
@@ -182,7 +248,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +291,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -238,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -250,6 +322,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -365,56 +441,47 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$27:$R$27</c:f>
+              <c:f>Sheet1!$C$26:$O$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1157,16 +1224,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>4152</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>4152</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1457,35 +1524,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="44.90625" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="11" max="11" width="11.1796875" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" customWidth="1"/>
+    <col min="15" max="15" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -1494,382 +1567,616 @@
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>3</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="C6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2">
+        <v>4</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4</v>
+      </c>
+      <c r="J8" s="2">
+        <v>4</v>
+      </c>
+      <c r="K8" s="2">
+        <v>4</v>
+      </c>
+      <c r="L8" s="2">
+        <v>4</v>
+      </c>
+      <c r="M8" s="2">
+        <v>4</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="C11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>5</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
+      <c r="K12" s="2">
+        <v>5</v>
+      </c>
+      <c r="L12" s="2">
+        <v>3</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="1">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D13" s="2">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="D14" s="2">
         <v>3</v>
       </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>3</v>
+      </c>
+      <c r="K14" s="2">
+        <v>3</v>
+      </c>
+      <c r="L14" s="2">
+        <v>3</v>
+      </c>
+      <c r="M14" s="2">
+        <v>3</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1882,11 +2189,8 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1902,11 +2206,8 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1922,11 +2223,8 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1942,11 +2240,8 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1962,11 +2257,8 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1982,11 +2274,8 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2002,11 +2291,8 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2022,11 +2308,8 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2042,11 +2325,8 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2062,11 +2342,8 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2082,253 +2359,460 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="4" t="s">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="3">
+        <f>SUM(C3:C25)</f>
+        <v>29</v>
+      </c>
+      <c r="D26" s="3">
+        <f>SUM(D3:D25)</f>
+        <v>29</v>
+      </c>
+      <c r="E26" s="3">
+        <f>SUM(E3:E25)</f>
+        <v>25</v>
+      </c>
+      <c r="F26" s="3">
+        <f>SUM(F3:F25)</f>
+        <v>21</v>
+      </c>
+      <c r="G26" s="3">
+        <f>SUM(G3:G25)</f>
+        <v>21</v>
+      </c>
+      <c r="H26" s="3">
+        <f t="shared" ref="H26:O26" si="0">SUM(H3:H25)</f>
+        <v>21</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" si="0"/>
+        <v>19.5</v>
+      </c>
+      <c r="L26" s="3">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
+      <c r="M26" s="3">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="N26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="10">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="10">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="10">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="10">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="10">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="10">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="10">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="10">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="10">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="10">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="10">
+        <v>5</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="3">
-        <f>SUM(C3:C26)</f>
-        <v>33</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="3">
-        <f t="shared" ref="H27:R27" si="1">SUM(H3:H26)</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="10" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="10">
         <v>1</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="D44" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="10">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C46" s="10">
+        <v>4</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="10">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="10">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="7"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="10"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="7"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="10"/>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="7"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="10"/>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="7"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="10"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="7"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C53" s="10"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="7"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C55" s="3">
-        <f>SUM(C31:C54)</f>
-        <v>0</v>
-      </c>
+      <c r="C54" s="10"/>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="7"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="7"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="7"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="7"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="7"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="7"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="7"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="1"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="7"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="7"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="1"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B64" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="3">
+        <f>SUM(C30:C63)</f>
+        <v>47.5</v>
+      </c>
+      <c r="D64" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>